<commit_message>
Class work and Homework
</commit_message>
<xml_diff>
--- a/3/Activities/01-Ins_BasicCharting/Solved/BasicCharts.xlsx
+++ b/3/Activities/01-Ins_BasicCharting/Solved/BasicCharts.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\OneDrive\Documents\WorkAndSchool\TeachingAssistant\DataViz\DataViz-Lesson-Plans\01-Lesson-Plans\01-Excel\3\Activities\02-Ins_BasicCharting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrettgomez/Desktop/RBootcamp/RBootcamp/3/Activities/01-Ins_BasicCharting/Solved/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="F83C7F0B9C5BB36C676B768E03FEC89EF1BFA6B5" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{F5E47B7C-E461-45D1-AFA9-F37C2DE297AD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393E7EF8-DF09-5F41-9C95-B2F805AD1BFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14610" windowHeight="14070" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33380" yWindow="2100" windowWidth="23140" windowHeight="14880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Favorite Ice Cream Flavors" sheetId="1" r:id="rId1"/>
     <sheet name="Ice Cream Sales" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Ice Cream Sales'!$A$1:$A$11</definedName>
+  </definedNames>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1342,6 +1345,14 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.36954855643044615"/>
+          <c:y val="6.4814814814814811E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1371,6 +1382,844 @@
         </a:p>
       </c:txPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Favorite Ice Cream Flavors'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Faves</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-F4F2-4543-9DEA-116FE6E87F9E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Favorite Ice Cream Flavors'!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Vanilla</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Chocolate</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Strawberry</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Mint</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Rocky Road</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Rainbow Sherbert</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Butter Pecan</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Cookie Dough</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Coffee</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Neapolitan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Favorite Ice Cream Flavors'!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F4F2-4543-9DEA-116FE6E87F9E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="979945184"/>
+        <c:axId val="1019723264"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="979945184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1019723264"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1019723264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="979945184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050">
+                  <a:alpha val="40000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-8D9F-4F40-81CB-139F8BC9D257}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Favorite Ice Cream Flavors'!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Vanilla</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Chocolate</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Strawberry</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Mint</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Rocky Road</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Rainbow Sherbert</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Butter Pecan</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Cookie Dough</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Coffee</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Neapolitan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Favorite Ice Cream Flavors'!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8D9F-4F40-81CB-139F8BC9D257}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1880,7 +2729,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$A$6</c15:sqref>
@@ -1909,7 +2758,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$B$1:$L$1</c15:sqref>
@@ -1956,7 +2805,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$B$6:$L$6</c15:sqref>
@@ -2003,7 +2852,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-8B0B-41D6-BCCA-6C2E7079979C}"/>
                   </c:ext>
@@ -2016,7 +2865,7 @@
                 <c:order val="5"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$A$7</c15:sqref>
@@ -2045,7 +2894,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$B$1:$L$1</c15:sqref>
@@ -2092,7 +2941,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$B$7:$L$7</c15:sqref>
@@ -2139,7 +2988,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-8B0B-41D6-BCCA-6C2E7079979C}"/>
                   </c:ext>
@@ -2152,7 +3001,7 @@
                 <c:order val="6"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$A$8</c15:sqref>
@@ -2183,7 +3032,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$B$1:$L$1</c15:sqref>
@@ -2230,7 +3079,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$B$8:$L$8</c15:sqref>
@@ -2277,7 +3126,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-8B0B-41D6-BCCA-6C2E7079979C}"/>
                   </c:ext>
@@ -2290,7 +3139,7 @@
                 <c:order val="7"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$A$9</c15:sqref>
@@ -2321,7 +3170,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$B$1:$L$1</c15:sqref>
@@ -2368,7 +3217,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$B$9:$L$9</c15:sqref>
@@ -2415,7 +3264,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-8B0B-41D6-BCCA-6C2E7079979C}"/>
                   </c:ext>
@@ -2428,7 +3277,7 @@
                 <c:order val="8"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$A$10</c15:sqref>
@@ -2459,7 +3308,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$B$1:$L$1</c15:sqref>
@@ -2506,7 +3355,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$B$10:$L$10</c15:sqref>
@@ -2553,7 +3402,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000008-8B0B-41D6-BCCA-6C2E7079979C}"/>
                   </c:ext>
@@ -2566,7 +3415,7 @@
                 <c:order val="9"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$A$11</c15:sqref>
@@ -2597,7 +3446,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$B$1:$L$1</c15:sqref>
@@ -2644,7 +3493,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$B$11:$L$11</c15:sqref>
@@ -2691,7 +3540,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000009-8B0B-41D6-BCCA-6C2E7079979C}"/>
                   </c:ext>
@@ -2884,6 +3733,1426 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ice Cream Sales'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vanilla</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ice Cream Sales'!$B$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ice Cream Sales'!$B$2:$L$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>247</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>306</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>301</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>350</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0BE9-EB45-B45D-04D9737DB74A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ice Cream Sales'!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Chocolate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ice Cream Sales'!$B$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ice Cream Sales'!$B$3:$L$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>243</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0BE9-EB45-B45D-04D9737DB74A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ice Cream Sales'!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Strawberry</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ice Cream Sales'!$B$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ice Cream Sales'!$B$4:$L$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>242</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>251</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0BE9-EB45-B45D-04D9737DB74A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ice Cream Sales'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mint</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ice Cream Sales'!$B$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ice Cream Sales'!$B$5:$L$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>163</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>254</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>292</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>318</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>373</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>386</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0BE9-EB45-B45D-04D9737DB74A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ice Cream Sales'!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rocky Road</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ice Cream Sales'!$B$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ice Cream Sales'!$B$6:$L$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>258</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>295</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>327</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>328</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>353</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>374</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>418</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>441</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>453</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-0BE9-EB45-B45D-04D9737DB74A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ice Cream Sales'!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rainbow Sherbert</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ice Cream Sales'!$B$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ice Cream Sales'!$B$7:$L$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>163</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>248</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>273</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-0BE9-EB45-B45D-04D9737DB74A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ice Cream Sales'!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Butter Pecan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ice Cream Sales'!$B$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ice Cream Sales'!$B$8:$L$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>123</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-0BE9-EB45-B45D-04D9737DB74A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ice Cream Sales'!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cookie Dough</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ice Cream Sales'!$B$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ice Cream Sales'!$B$9:$L$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>163</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>202</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-0BE9-EB45-B45D-04D9737DB74A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ice Cream Sales'!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Coffee</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ice Cream Sales'!$B$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ice Cream Sales'!$B$10:$L$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>198</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-0BE9-EB45-B45D-04D9737DB74A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ice Cream Sales'!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Neapolitan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ice Cream Sales'!$B$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ice Cream Sales'!$B$11:$L$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-0BE9-EB45-B45D-04D9737DB74A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="412007055"/>
+        <c:axId val="440310783"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="412007055"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="440310783"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="440310783"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="412007055"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3004,6 +5273,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="212">
   <cs:axisTitle>
@@ -4024,6 +6413,1544 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4613,6 +8540,78 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>965200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C788A41-6FDB-7142-A5FD-FCF30671661F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>889000</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42A0E75F-2306-B74B-AFDC-1FEFE2ED04E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4649,6 +8648,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE74295C-59B7-5F4D-81D8-5BBE06C6C26E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4956,16 +8991,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" activeCellId="2" sqref="A1 A1:A11 C1:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="8" width="20.73046875" customWidth="1"/>
+    <col min="1" max="8" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -4978,7 +9013,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4990,7 +9025,7 @@
         <v>0.11166666666666666</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -5002,7 +9037,7 @@
         <v>8.8333333333333333E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -5014,7 +9049,7 @@
         <v>0.10666666666666667</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -5026,7 +9061,7 @@
         <v>0.15666666666666668</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -5038,7 +9073,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -5050,7 +9085,7 @@
         <v>0.13166666666666665</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -5062,7 +9097,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -5074,7 +9109,7 @@
         <v>6.8333333333333329E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -5086,7 +9121,7 @@
         <v>5.6666666666666664E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -5098,12 +9133,12 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <f>SUM(B2:B11)</f>
         <v>600</v>
@@ -5120,17 +9155,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.73046875" customWidth="1"/>
-    <col min="2" max="8" width="8.73046875" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="8" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>14</v>
       </c>
@@ -5165,7 +9200,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -5203,7 +9238,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -5241,7 +9276,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -5279,7 +9314,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -5317,7 +9352,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -5355,7 +9390,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -5393,7 +9428,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -5431,7 +9466,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -5469,7 +9504,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -5507,7 +9542,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -5546,6 +9581,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A11" xr:uid="{B98CFB3B-B0C1-5D41-82C0-79F56D9D8470}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>